<commit_message>
Complexity rubric update notes
</commit_message>
<xml_diff>
--- a/proposal/complexity-rubric.xlsx
+++ b/proposal/complexity-rubric.xlsx
@@ -1,17 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\CS447-Project-2\proposal\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB2669D-955F-4F3E-99E1-92C1BA1DD40E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="2565" yWindow="1125" windowWidth="23700" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Project 2 Complexity " sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - Project 2 Complexity " sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Project 2 Complexity Rubric</t>
   </si>
@@ -80,15 +99,30 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Worms Type</t>
+  </si>
+  <si>
+    <t>2d zelda-like platformer</t>
+  </si>
+  <si>
+    <t>Contra</t>
+  </si>
+  <si>
+    <t>Tetris A-symetric VS platformer</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>!!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -101,7 +135,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -127,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -240,56 +274,187 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="24">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -300,26 +465,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -518,7 +742,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -537,7 +761,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -567,7 +791,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -593,7 +817,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -619,7 +843,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -645,7 +869,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -671,7 +895,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -697,7 +921,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -723,7 +947,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -749,7 +973,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -775,7 +999,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -788,9 +1012,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -807,7 +1037,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -826,7 +1056,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -852,7 +1082,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -878,7 +1108,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -904,7 +1134,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -930,7 +1160,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -956,7 +1186,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -982,7 +1212,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1008,7 +1238,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1034,7 +1264,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1060,7 +1290,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1073,9 +1303,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1089,7 +1325,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1108,7 +1344,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1138,7 +1374,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1164,7 +1400,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1190,7 +1426,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1216,7 +1452,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1242,7 +1478,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1268,7 +1504,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1294,7 +1530,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1320,7 +1556,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1346,7 +1582,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1359,415 +1595,566 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.2031" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.9297" style="1" customWidth="1"/>
-    <col min="5" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.9375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+    <col min="5" max="6" width="16.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:11" ht="27.6" customHeight="1" thickBot="1">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" t="s" s="3">
+      <c r="B2" s="3"/>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="H2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>20</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <f>B3</f>
         <v>20</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <f>B3</f>
         <v>20</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <f>B3</f>
         <v>20</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="7">
+      <c r="F3" s="7"/>
+      <c r="G3" s="16">
         <f>B3</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="9">
+      <c r="H3" s="21">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>30</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <f>B4</f>
         <v>30</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="11">
+      <c r="D4" s="11"/>
+      <c r="E4" s="10">
         <f>B4</f>
         <v>30</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="9">
+      <c r="F4" s="11"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="21">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>15</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <f>B5</f>
         <v>15</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <f>B5</f>
         <v>15</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <f>B5</f>
         <v>15</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="B6" s="10">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11">
+      <c r="F5" s="11"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="21">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1">
+        <v>15</v>
+      </c>
+      <c r="J5" s="1">
+        <v>15</v>
+      </c>
+      <c r="K5" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10">
         <f>B6</f>
         <v>10</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="11">
+      <c r="D6" s="11"/>
+      <c r="E6" s="10">
         <f>B6</f>
         <v>10</v>
       </c>
-      <c r="F6" s="11">
-        <v>10</v>
-      </c>
-      <c r="G6" s="11">
+      <c r="F6" s="10">
+        <v>10</v>
+      </c>
+      <c r="G6" s="18">
         <f>B6</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="9">
+      <c r="H6" s="21">
+        <v>10</v>
+      </c>
+      <c r="I6" s="1">
+        <v>10</v>
+      </c>
+      <c r="J6" s="1">
+        <v>10</v>
+      </c>
+      <c r="K6" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>50</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11">
+      <c r="C7" s="11"/>
+      <c r="D7" s="10">
         <f>B7</f>
         <v>50</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="9">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>25</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="11">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="10">
         <v>25</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="18">
         <f>B8</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="9">
+      <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>55</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="9">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="10">
-        <v>10</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="11">
+      <c r="B10" s="9">
+        <v>10</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10">
         <f>B10</f>
         <v>10</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="9">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="17">
+        <v>10</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="J10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>20</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <f>B11</f>
         <v>20</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="11">
+      <c r="D11" s="11"/>
+      <c r="E11" s="10">
         <v>20</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="9">
+      <c r="F11" s="11"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="21">
+        <v>20</v>
+      </c>
+      <c r="I11" s="1">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="10">
-        <v>10</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="11">
+      <c r="B12" s="9">
+        <v>10</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10">
         <f>B12</f>
         <v>10</v>
       </c>
-      <c r="E12" s="11">
-        <v>10</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="9">
+      <c r="E12" s="10">
+        <v>10</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="17">
+        <v>10</v>
+      </c>
+      <c r="H12" s="21">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1">
+        <v>10</v>
+      </c>
+      <c r="K12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>20</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <f>B13</f>
         <v>20</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="9">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>25</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="11">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="10">
         <v>25</v>
       </c>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="9">
+      <c r="G14" s="17"/>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="10">
-        <v>10</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="9">
+      <c r="B15" s="9">
+        <v>10</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="1">
         <v>20</v>
       </c>
-      <c r="B16" s="10">
+      <c r="H15" s="21"/>
+      <c r="I15" s="1">
+        <v>10</v>
+      </c>
+      <c r="J15" s="1">
+        <v>10</v>
+      </c>
+      <c r="K15" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="9">
+      <c r="B16" s="9">
+        <v>20</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="10">
-        <v>10</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="11">
+      <c r="B17" s="9">
+        <v>10</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="10">
         <f>B17</f>
         <v>10</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="9">
+      <c r="F17" s="11"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="21"/>
+    </row>
+    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <f>SUM(B3:B18)</f>
         <v>330</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <f>SUM(C3:C18)</f>
         <v>115</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="10">
         <f>SUM(D3:D18)</f>
         <v>105</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <f>SUM(E3:E18)</f>
         <v>115</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <f>SUM(F3:F18)</f>
         <v>60</v>
       </c>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="G19" s="18">
+        <f>SUM(G3:G18)</f>
+        <v>95</v>
+      </c>
+      <c r="H19" s="22">
+        <f>SUM(H3:H18)</f>
+        <v>125</v>
+      </c>
+      <c r="I19" s="19">
+        <f>SUM(I3:I18)</f>
+        <v>115</v>
+      </c>
+      <c r="J19" s="10">
+        <f t="shared" ref="J19:K19" si="0">SUM(J3:J18)</f>
+        <v>105</v>
+      </c>
+      <c r="K19" s="10">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>